<commit_message>
refacto: labels et import
</commit_message>
<xml_diff>
--- a/packages/frontend/src/assets/files/modele_import_domifa.xlsx
+++ b/packages/frontend/src/assets/files/modele_import_domifa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/frontend/src/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B83577-7715-3D40-8542-F530BBBB4F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C6ED6C-F303-3049-BEDB-711F8A6CA657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3030,7 +3030,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X4" sqref="X4"/>
+      <selection pane="bottomLeft" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
test(import): Ajout de tests sur l'import des domiciliés fix(import): Correction d'un bug sur les dates de dernier passage fix(dossier): Correction de l'affichage des titres
</commit_message>
<xml_diff>
--- a/packages/frontend/src/assets/files/modele_import_domifa.xlsx
+++ b/packages/frontend/src/assets/files/modele_import_domifa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/frontend/src/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C6ED6C-F303-3049-BEDB-711F8A6CA657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE414A67-622F-6445-BFCA-E1359A4FBD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOMICILIES" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="155">
   <si>
     <t>Civilité</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Type de domiciliation</t>
-  </si>
-  <si>
-    <t>Date début dom actuelle</t>
   </si>
   <si>
     <t>Date 1ere domiciliation</t>
@@ -217,9 +214,6 @@
   </si>
   <si>
     <t>SATURATION</t>
-  </si>
-  <si>
-    <t>12/09/2019</t>
   </si>
   <si>
     <t>09/08/2020</t>
@@ -759,12 +753,48 @@
   <si>
     <t>SOCIAL</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Seulement si valide</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12.5"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Date début dom actuelle</t>
+    </r>
+  </si>
+  <si>
+    <t>PREMIERE_DOM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -936,6 +966,14 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1112,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1224,53 +1262,14 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="58">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2023,6 +2022,48 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2786,7 +2827,7 @@
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Seulement si refus_x000a_Motif du refus" dataDxfId="39"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Seulement si radié_x000a_Motif de radiation" dataDxfId="38"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Type de domiciliation" dataDxfId="37"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Date début dom actuelle" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Seulement si valide_x000a_Date début dom actuelle" dataDxfId="36"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Date de fin de domiciliation_x000a_OU_x000a_Date de radiation si radié_x000a_OU _x000a_Date de refus si refusé" dataDxfId="35"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Date 1ere domiciliation" dataDxfId="34"/>
     <tableColumn id="13" xr3:uid="{F3EC0B77-5925-4549-B090-3175E9AD69D3}" name="Date de dernier passage _x000a_(si vide, la date sera celle de l'import)" dataDxfId="33"/>
@@ -2796,33 +2837,33 @@
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="La personne a-t-elle des revenus ?" dataDxfId="29"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Seulement si revenus_x000a_De quelle nature ?" dataDxfId="28"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Quel est le lien avec la commune ? _x000a_(Si CCAS ou CIAS)" dataDxfId="27"/>
-    <tableColumn id="51" xr3:uid="{04744227-FC84-8F43-9683-A1C7B78F5FB9}" name="Si AUTRE lien avec la commune_x000a_précisions" dataDxfId="0"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Composition du ménage" dataDxfId="26"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Situation résidentielle" dataDxfId="25"/>
-    <tableColumn id="45" xr3:uid="{973BA99D-2099-8447-A5F6-C95462E9533B}" name="Si AUTRE situation résidentielle_x000a_précisions" dataDxfId="24"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Cause de l'instabilité_x000a_ du logement" dataDxfId="23"/>
-    <tableColumn id="46" xr3:uid="{CAFD5E43-FC29-714C-BEA8-B5320362468C}" name="Si AUTRE cause d'instabilité_x000a_précisions" dataDxfId="22"/>
-    <tableColumn id="48" xr3:uid="{8A6DC35C-929D-2341-AFBA-85F886983314}" name="Quel est le motif principal de demande de domiciliation ?" dataDxfId="21"/>
-    <tableColumn id="47" xr3:uid="{A55284FD-ADFF-1848-88BD-250C0B85E5E4}" name="Si AUTRE motif,_x000a_précisions" dataDxfId="20"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Accompagnement social" dataDxfId="19"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Seulement si accompagnement_x000a_Par quelle structure est fait l'accompagnement?" dataDxfId="18"/>
-    <tableColumn id="49" xr3:uid="{2432BDAC-54A8-974C-BD03-3795C92EFD8C}" name="Commentaires _x000a_(1000 caractères maximum)" dataDxfId="17"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Nom Ayant-Droit 1" dataDxfId="16"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Prénom Ayant-Droit 1" dataDxfId="15"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Date de Naissance Ayant-Droit 1" dataDxfId="14"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Lien de parenté Ayant-Droit 1" dataDxfId="13"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Nom Ayant-Droit 2" dataDxfId="12"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Prénom Ayant-Droit 2" dataDxfId="11"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Date de Naissance Ayant-Droit 2" dataDxfId="10"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Lien de parenté Ayant-Droit 2" dataDxfId="9"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Nom Ayant-Droit 3" dataDxfId="8"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Prénom Ayant-Droit 3" dataDxfId="7"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Date de Naissance_x000a_Ayant-Droit 3" dataDxfId="6"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Lien de parenté_x000a_Ayant-Droit 3" dataDxfId="5"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Nom Ayant-Droit 4" dataDxfId="4"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Prénom Ayant-Droit 4" dataDxfId="3"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Date de Naissance Ayant-Droit 4" dataDxfId="2"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Lien de parenté Ayant-Droit 4" dataDxfId="1"/>
+    <tableColumn id="51" xr3:uid="{04744227-FC84-8F43-9683-A1C7B78F5FB9}" name="Si AUTRE lien avec la commune_x000a_précisions" dataDxfId="26"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Composition du ménage" dataDxfId="25"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Situation résidentielle" dataDxfId="24"/>
+    <tableColumn id="45" xr3:uid="{973BA99D-2099-8447-A5F6-C95462E9533B}" name="Si AUTRE situation résidentielle_x000a_précisions" dataDxfId="23"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Cause de l'instabilité_x000a_ du logement" dataDxfId="22"/>
+    <tableColumn id="46" xr3:uid="{CAFD5E43-FC29-714C-BEA8-B5320362468C}" name="Si AUTRE cause d'instabilité_x000a_précisions" dataDxfId="21"/>
+    <tableColumn id="48" xr3:uid="{8A6DC35C-929D-2341-AFBA-85F886983314}" name="Quel est le motif principal de demande de domiciliation ?" dataDxfId="20"/>
+    <tableColumn id="47" xr3:uid="{A55284FD-ADFF-1848-88BD-250C0B85E5E4}" name="Si AUTRE motif,_x000a_précisions" dataDxfId="19"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Accompagnement social" dataDxfId="18"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Seulement si accompagnement_x000a_Par quelle structure est fait l'accompagnement?" dataDxfId="17"/>
+    <tableColumn id="49" xr3:uid="{2432BDAC-54A8-974C-BD03-3795C92EFD8C}" name="Commentaires _x000a_(1000 caractères maximum)" dataDxfId="16"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Nom Ayant-Droit 1" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Prénom Ayant-Droit 1" dataDxfId="14"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Date de Naissance Ayant-Droit 1" dataDxfId="13"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Lien de parenté Ayant-Droit 1" dataDxfId="12"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Nom Ayant-Droit 2" dataDxfId="11"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Prénom Ayant-Droit 2" dataDxfId="10"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Date de Naissance Ayant-Droit 2" dataDxfId="9"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Lien de parenté Ayant-Droit 2" dataDxfId="8"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Nom Ayant-Droit 3" dataDxfId="7"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Prénom Ayant-Droit 3" dataDxfId="6"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Date de Naissance_x000a_Ayant-Droit 3" dataDxfId="5"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Lien de parenté_x000a_Ayant-Droit 3" dataDxfId="4"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Nom Ayant-Droit 4" dataDxfId="3"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Prénom Ayant-Droit 4" dataDxfId="2"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Date de Naissance Ayant-Droit 4" dataDxfId="1"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Lien de parenté Ayant-Droit 4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="DOMICILIES-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3028,15 +3069,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1"/>
@@ -3070,7 +3111,7 @@
   <sheetData>
     <row r="1" spans="1:50" s="19" customFormat="1" ht="116" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -3100,236 +3141,236 @@
         <v>8</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="Q1" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="T1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="X1" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="16" t="s">
-        <v>127</v>
+      <c r="Z1" s="16" t="s">
+        <v>12</v>
       </c>
-      <c r="R1" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" s="16" t="s">
+      <c r="AA1" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="AB1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG1" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="U1" s="16" t="s">
-        <v>131</v>
+      <c r="AH1" s="17" t="s">
+        <v>126</v>
       </c>
-      <c r="V1" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="W1" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="X1" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AI1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="17" t="s">
+      <c r="AJ1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX1" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="AH1" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="AI1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="AO1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="AP1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="AQ1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="AS1" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="AT1" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="AU1" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="AV1" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="AW1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="AX1" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>143</v>
-      </c>
       <c r="B2" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="J2" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="O2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="P2" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="X2" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="Y2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="21" t="s">
-        <v>146</v>
+      <c r="Z2" s="24" t="s">
+        <v>95</v>
       </c>
-      <c r="Q2" s="21" t="s">
-        <v>114</v>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25" t="s">
+        <v>86</v>
       </c>
-      <c r="R2" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="W2" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="X2" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
       <c r="AE2" s="24"/>
       <c r="AF2" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AG2" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AH2" s="22"/>
       <c r="AI2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="22" t="s">
+      <c r="AK2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="AK2" s="22" t="s">
+      <c r="AL2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="AL2" s="22" t="s">
+      <c r="AM2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN2" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="AM2" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN2" s="22" t="s">
+      <c r="AO2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="AO2" s="22" t="s">
-        <v>45</v>
-      </c>
       <c r="AP2" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AQ2" s="22"/>
       <c r="AR2" s="22"/>
@@ -3342,100 +3383,100 @@
     </row>
     <row r="3" spans="1:50" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>51</v>
-      </c>
       <c r="J3" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
       <c r="M3" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="Q3" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="S3" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="21" t="s">
-        <v>54</v>
+      <c r="T3" s="21" t="s">
+        <v>92</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="U3" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="V3" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="R3" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="S3" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="V3" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="W3" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="X3" s="22"/>
       <c r="Y3" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Z3" s="24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
-      <c r="AA3" s="24"/>
+      <c r="AA3" s="25"/>
       <c r="AB3" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="22" t="s">
-        <v>108</v>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="AE3" s="22"/>
       <c r="AF3" s="21"/>
       <c r="AG3" s="22"/>
       <c r="AH3" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AI3" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AJ3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AK3" s="22" t="s">
+      <c r="AL3" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="AL3" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="AM3" s="22"/>
       <c r="AN3" s="22"/>
@@ -3452,43 +3493,41 @@
     </row>
     <row r="4" spans="1:50" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="21"/>
       <c r="I4" s="27"/>
       <c r="J4" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
-      <c r="N4" s="21" t="s">
-        <v>63</v>
-      </c>
+      <c r="N4" s="21"/>
       <c r="O4" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
@@ -3496,38 +3535,38 @@
       <c r="S4" s="22"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
       <c r="X4" s="22"/>
       <c r="Y4" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
-      <c r="AA4" s="24" t="s">
+      <c r="AA4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE4" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF4" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG4" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="AB4" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE4" s="22" t="s">
+      <c r="AH4" s="22" t="s">
         <v>118</v>
-      </c>
-      <c r="AF4" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG4" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="AH4" s="22" t="s">
-        <v>120</v>
       </c>
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
@@ -55388,8 +55427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -55403,133 +55442,133 @@
     <col min="7" max="7" width="36.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="30.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="26" width="10.5703125" style="1" customWidth="1"/>
     <col min="27" max="16384" width="11.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>103</v>
+      <c r="F2" s="9" t="s">
+        <v>63</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>100</v>
+      <c r="H2" s="9" t="s">
+        <v>83</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>13</v>
+      <c r="I2" s="9" t="s">
+        <v>93</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J2" s="35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J3" s="35" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>108</v>
-      </c>
-    </row>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -55537,89 +55576,89 @@
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -55627,14 +55666,14 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -55646,7 +55685,7 @@
     <row r="11" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -55657,18 +55696,18 @@
     </row>
     <row r="12" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G14" s="2"/>
     </row>

</xml_diff>